<commit_message>
Update to main pages
</commit_message>
<xml_diff>
--- a/reaction_time_cleaned.xlsx
+++ b/reaction_time_cleaned.xlsx
@@ -1,20 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d8cf09cc5c81962a/School/ABE 516x/516x-master/Final/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_F766B041F6E213C300424FAF23A9541160B52A82" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4F7E4DA-AA0C-438C-BA44-672B88B97DF7}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="38280" yWindow="-2730" windowWidth="16440" windowHeight="28440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="Class Activity" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1839" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1854" uniqueCount="28">
   <si>
     <t>sex</t>
   </si>
@@ -103,8 +110,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,6 +174,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -213,7 +228,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -245,9 +260,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -279,6 +312,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -454,14 +505,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I306"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:I4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -490,7 +543,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -516,10 +569,10 @@
         <v>23</v>
       </c>
       <c r="I2">
-        <v>0.325</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>0.32500000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -545,10 +598,10 @@
         <v>23</v>
       </c>
       <c r="I3">
-        <v>0.33199</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>0.33199000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -574,10 +627,10 @@
         <v>23</v>
       </c>
       <c r="I4">
-        <v>0.298999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>0.29899900000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -603,10 +656,10 @@
         <v>23</v>
       </c>
       <c r="I5">
-        <v>0.3619999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>0.36199989999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -632,10 +685,10 @@
         <v>23</v>
       </c>
       <c r="I6">
-        <v>0.328999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+        <v>0.32899899999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -661,10 +714,10 @@
         <v>23</v>
       </c>
       <c r="I7">
-        <v>0.306999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <v>0.30699900000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -690,10 +743,10 @@
         <v>23</v>
       </c>
       <c r="I8">
-        <v>0.529</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+        <v>0.52900000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -719,10 +772,10 @@
         <v>23</v>
       </c>
       <c r="I9">
-        <v>0.498999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>0.49899900000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -751,7 +804,7 @@
         <v>1.599</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -777,10 +830,10 @@
         <v>23</v>
       </c>
       <c r="I11">
-        <v>0.448999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+        <v>0.44899899999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -806,10 +859,10 @@
         <v>23</v>
       </c>
       <c r="I12">
-        <v>0.332</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+        <v>0.33200000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -835,10 +888,10 @@
         <v>23</v>
       </c>
       <c r="I13">
-        <v>0.362</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+        <v>0.36199999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -864,10 +917,10 @@
         <v>23</v>
       </c>
       <c r="I14">
-        <v>0.391</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+        <v>0.39100000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -893,10 +946,10 @@
         <v>23</v>
       </c>
       <c r="I15">
-        <v>0.391</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+        <v>0.39100000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -922,10 +975,10 @@
         <v>23</v>
       </c>
       <c r="I16">
-        <v>0.455</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
+        <v>0.45500000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -951,10 +1004,10 @@
         <v>23</v>
       </c>
       <c r="I17">
-        <v>0.706999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
+        <v>0.70699900000000004</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -980,10 +1033,10 @@
         <v>23</v>
       </c>
       <c r="I18">
-        <v>0.955999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
+        <v>0.95599900000000004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -1012,7 +1065,7 @@
         <v>1.454</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -1038,10 +1091,10 @@
         <v>23</v>
       </c>
       <c r="I20">
-        <v>0.429</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
+        <v>0.42899999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -1067,10 +1120,10 @@
         <v>23</v>
       </c>
       <c r="I21">
-        <v>0.428999</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
+        <v>0.42899900000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -1096,10 +1149,10 @@
         <v>23</v>
       </c>
       <c r="I22">
-        <v>0.363999</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
+        <v>0.36399900000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -1125,10 +1178,10 @@
         <v>23</v>
       </c>
       <c r="I23">
-        <v>0.429</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
+        <v>0.42899999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -1154,10 +1207,10 @@
         <v>23</v>
       </c>
       <c r="I24">
-        <v>0.428999</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
+        <v>0.42899900000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>10</v>
       </c>
@@ -1183,10 +1236,10 @@
         <v>23</v>
       </c>
       <c r="I25">
-        <v>0.363999</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
+        <v>0.36399900000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -1212,10 +1265,10 @@
         <v>23</v>
       </c>
       <c r="I26">
-        <v>0.306999</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
+        <v>0.30699900000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -1244,7 +1297,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -1270,10 +1323,10 @@
         <v>23</v>
       </c>
       <c r="I28">
-        <v>0.400999</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
+        <v>0.40099899999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -1299,10 +1352,10 @@
         <v>23</v>
       </c>
       <c r="I29">
-        <v>0.4579</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
+        <v>0.45789999999999997</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>9</v>
       </c>
@@ -1331,7 +1384,7 @@
         <v>0.314</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -1360,7 +1413,7 @@
         <v>0.3589</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -1386,10 +1439,10 @@
         <v>23</v>
       </c>
       <c r="I32">
-        <v>0.458</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9">
+        <v>0.45800000000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -1415,10 +1468,10 @@
         <v>23</v>
       </c>
       <c r="I33">
-        <v>0.359</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9">
+        <v>0.35899999999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>10</v>
       </c>
@@ -1444,10 +1497,10 @@
         <v>23</v>
       </c>
       <c r="I34">
-        <v>0.327</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
+        <v>0.32700000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>9</v>
       </c>
@@ -1473,10 +1526,10 @@
         <v>23</v>
       </c>
       <c r="I35">
-        <v>0.3969</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9">
+        <v>0.39689999999999998</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>9</v>
       </c>
@@ -1505,7 +1558,7 @@
         <v>0.2319</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>9</v>
       </c>
@@ -1531,10 +1584,10 @@
         <v>23</v>
       </c>
       <c r="I37">
-        <v>0.4009</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9">
+        <v>0.40089999999999998</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>10</v>
       </c>
@@ -1560,10 +1613,10 @@
         <v>23</v>
       </c>
       <c r="I38">
-        <v>0.3919</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9">
+        <v>0.39190000000000003</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>10</v>
       </c>
@@ -1589,10 +1642,10 @@
         <v>23</v>
       </c>
       <c r="I39">
-        <v>0.2599</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9">
+        <v>0.25990000000000002</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>10</v>
       </c>
@@ -1618,10 +1671,10 @@
         <v>23</v>
       </c>
       <c r="I40">
-        <v>0.425</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9">
+        <v>0.42499999999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>9</v>
       </c>
@@ -1650,7 +1703,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>9</v>
       </c>
@@ -1676,10 +1729,10 @@
         <v>23</v>
       </c>
       <c r="I42">
-        <v>0.492</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9">
+        <v>0.49199999999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>9</v>
       </c>
@@ -1705,10 +1758,10 @@
         <v>23</v>
       </c>
       <c r="I43">
-        <v>0.299</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9">
+        <v>0.29899999999999999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>10</v>
       </c>
@@ -1734,10 +1787,10 @@
         <v>23</v>
       </c>
       <c r="I44">
-        <v>0.3249</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9">
+        <v>0.32490000000000002</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>10</v>
       </c>
@@ -1763,10 +1816,10 @@
         <v>23</v>
       </c>
       <c r="I45">
-        <v>0.358</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9">
+        <v>0.35799999999999998</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>10</v>
       </c>
@@ -1792,10 +1845,10 @@
         <v>23</v>
       </c>
       <c r="I46">
-        <v>0.358</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9">
+        <v>0.35799999999999998</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>9</v>
       </c>
@@ -1821,10 +1874,10 @@
         <v>23</v>
       </c>
       <c r="I47">
-        <v>0.033</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9">
+        <v>3.3000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>9</v>
       </c>
@@ -1850,10 +1903,10 @@
         <v>23</v>
       </c>
       <c r="I48">
-        <v>0.295999</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9">
+        <v>0.29599900000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>9</v>
       </c>
@@ -1882,7 +1935,7 @@
         <v>0.503</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>9</v>
       </c>
@@ -1908,10 +1961,10 @@
         <v>23</v>
       </c>
       <c r="I50">
-        <v>0.692999</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9">
+        <v>0.69299900000000003</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>9</v>
       </c>
@@ -1937,10 +1990,10 @@
         <v>23</v>
       </c>
       <c r="I51">
-        <v>1.035999</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9">
+        <v>1.0359989999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>9</v>
       </c>
@@ -1966,10 +2019,10 @@
         <v>23</v>
       </c>
       <c r="I52">
-        <v>0.397</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9">
+        <v>0.39700000000000002</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>10</v>
       </c>
@@ -1995,10 +2048,10 @@
         <v>23</v>
       </c>
       <c r="I53">
-        <v>2.376</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9">
+        <v>2.3759999999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>10</v>
       </c>
@@ -2024,10 +2077,10 @@
         <v>23</v>
       </c>
       <c r="I54">
-        <v>0.493999</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9">
+        <v>0.49399900000000002</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>10</v>
       </c>
@@ -2053,10 +2106,10 @@
         <v>23</v>
       </c>
       <c r="I55">
-        <v>0.493999</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9">
+        <v>0.49399900000000002</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>10</v>
       </c>
@@ -2082,10 +2135,10 @@
         <v>23</v>
       </c>
       <c r="I56">
-        <v>0.631</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9">
+        <v>0.63100000000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>9</v>
       </c>
@@ -2111,10 +2164,10 @@
         <v>23</v>
       </c>
       <c r="I57">
-        <v>0.362</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9">
+        <v>0.36199999999999999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>9</v>
       </c>
@@ -2140,10 +2193,10 @@
         <v>23</v>
       </c>
       <c r="I58">
-        <v>0.595909</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9">
+        <v>0.59590900000000002</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>9</v>
       </c>
@@ -2172,7 +2225,7 @@
         <v>0.505</v>
       </c>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>10</v>
       </c>
@@ -2198,10 +2251,10 @@
         <v>23</v>
       </c>
       <c r="I60">
-        <v>0.493999</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9">
+        <v>0.49399900000000002</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>10</v>
       </c>
@@ -2227,10 +2280,10 @@
         <v>23</v>
       </c>
       <c r="I61">
-        <v>0.488999</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9">
+        <v>0.48899900000000002</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>10</v>
       </c>
@@ -2256,10 +2309,10 @@
         <v>23</v>
       </c>
       <c r="I62">
-        <v>0.651</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9">
+        <v>0.65100000000000002</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>9</v>
       </c>
@@ -2285,10 +2338,10 @@
         <v>24</v>
       </c>
       <c r="I63">
-        <v>0.267</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9">
+        <v>0.26700000000000002</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>9</v>
       </c>
@@ -2314,10 +2367,10 @@
         <v>24</v>
       </c>
       <c r="I64">
-        <v>0.232999</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9">
+        <v>0.23299900000000001</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>9</v>
       </c>
@@ -2346,7 +2399,7 @@
         <v>0.26599</v>
       </c>
     </row>
-    <row r="66" spans="1:9">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>9</v>
       </c>
@@ -2372,10 +2425,10 @@
         <v>24</v>
       </c>
       <c r="I66">
-        <v>0.3219999</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9">
+        <v>0.32199990000000001</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>9</v>
       </c>
@@ -2401,10 +2454,10 @@
         <v>24</v>
       </c>
       <c r="I67">
-        <v>0.331</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9">
+        <v>0.33100000000000002</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>9</v>
       </c>
@@ -2430,10 +2483,10 @@
         <v>24</v>
       </c>
       <c r="I68">
-        <v>0.363999</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9">
+        <v>0.36399900000000002</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>9</v>
       </c>
@@ -2459,10 +2512,10 @@
         <v>24</v>
       </c>
       <c r="I69">
-        <v>0.362999</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9">
+        <v>0.36299900000000002</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>9</v>
       </c>
@@ -2488,10 +2541,10 @@
         <v>24</v>
       </c>
       <c r="I70">
-        <v>0.396999</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9">
+        <v>0.39699899999999999</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>9</v>
       </c>
@@ -2517,10 +2570,10 @@
         <v>24</v>
       </c>
       <c r="I71">
-        <v>0.362999</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9">
+        <v>0.36299900000000002</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>10</v>
       </c>
@@ -2546,10 +2599,10 @@
         <v>24</v>
       </c>
       <c r="I72">
-        <v>0.461999</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9">
+        <v>0.46199899999999999</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>10</v>
       </c>
@@ -2575,10 +2628,10 @@
         <v>24</v>
       </c>
       <c r="I73">
-        <v>0.429</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9">
+        <v>0.42899999999999999</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>10</v>
       </c>
@@ -2604,10 +2657,10 @@
         <v>24</v>
       </c>
       <c r="I74">
-        <v>0.361</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9">
+        <v>0.36099999999999999</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>10</v>
       </c>
@@ -2633,10 +2686,10 @@
         <v>24</v>
       </c>
       <c r="I75">
-        <v>0.329</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9">
+        <v>0.32900000000000001</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>10</v>
       </c>
@@ -2662,10 +2715,10 @@
         <v>24</v>
       </c>
       <c r="I76">
-        <v>0.329</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9">
+        <v>0.32900000000000001</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>10</v>
       </c>
@@ -2691,10 +2744,10 @@
         <v>24</v>
       </c>
       <c r="I77">
-        <v>0.297</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9">
+        <v>0.29699999999999999</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>9</v>
       </c>
@@ -2720,10 +2773,10 @@
         <v>24</v>
       </c>
       <c r="I78">
-        <v>0.362999</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9">
+        <v>0.36299900000000002</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>9</v>
       </c>
@@ -2749,10 +2802,10 @@
         <v>24</v>
       </c>
       <c r="I79">
-        <v>0.295999</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9">
+        <v>0.29599900000000001</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>9</v>
       </c>
@@ -2778,10 +2831,10 @@
         <v>24</v>
       </c>
       <c r="I80">
-        <v>0.397</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9">
+        <v>0.39700000000000002</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>10</v>
       </c>
@@ -2807,10 +2860,10 @@
         <v>24</v>
       </c>
       <c r="I81">
-        <v>0.362999</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9">
+        <v>0.36299900000000002</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>10</v>
       </c>
@@ -2836,10 +2889,10 @@
         <v>24</v>
       </c>
       <c r="I82">
-        <v>0.463999</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9">
+        <v>0.46399899999999999</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>10</v>
       </c>
@@ -2865,10 +2918,10 @@
         <v>24</v>
       </c>
       <c r="I83">
-        <v>0.463</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9">
+        <v>0.46300000000000002</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>10</v>
       </c>
@@ -2894,10 +2947,10 @@
         <v>24</v>
       </c>
       <c r="I84">
-        <v>0.362999</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9">
+        <v>0.36299900000000002</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>10</v>
       </c>
@@ -2923,10 +2976,10 @@
         <v>24</v>
       </c>
       <c r="I85">
-        <v>0.463999</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9">
+        <v>0.46399899999999999</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>10</v>
       </c>
@@ -2952,10 +3005,10 @@
         <v>24</v>
       </c>
       <c r="I86">
-        <v>0.463</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9">
+        <v>0.46300000000000002</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>10</v>
       </c>
@@ -2981,10 +3034,10 @@
         <v>24</v>
       </c>
       <c r="I87">
-        <v>0.299999</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9">
+        <v>0.29999900000000002</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>10</v>
       </c>
@@ -3010,10 +3063,10 @@
         <v>24</v>
       </c>
       <c r="I88">
-        <v>0.361999</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9">
+        <v>0.36199900000000002</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>10</v>
       </c>
@@ -3039,10 +3092,10 @@
         <v>24</v>
       </c>
       <c r="I89">
-        <v>0.362</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9">
+        <v>0.36199999999999999</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>9</v>
       </c>
@@ -3068,10 +3121,10 @@
         <v>24</v>
       </c>
       <c r="I90">
-        <v>0.3329</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9">
+        <v>0.33289999999999997</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>9</v>
       </c>
@@ -3097,10 +3150,10 @@
         <v>24</v>
       </c>
       <c r="I91">
-        <v>0.2249</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9">
+        <v>0.22489999999999999</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>9</v>
       </c>
@@ -3126,10 +3179,10 @@
         <v>24</v>
       </c>
       <c r="I92">
-        <v>0.2759</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9">
+        <v>0.27589999999999998</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>10</v>
       </c>
@@ -3155,10 +3208,10 @@
         <v>24</v>
       </c>
       <c r="I93">
-        <v>0.3979</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9">
+        <v>0.39789999999999998</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>10</v>
       </c>
@@ -3184,10 +3237,10 @@
         <v>24</v>
       </c>
       <c r="I94">
-        <v>0.2599</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9">
+        <v>0.25990000000000002</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>10</v>
       </c>
@@ -3216,7 +3269,7 @@
         <v>0.3589</v>
       </c>
     </row>
-    <row r="96" spans="1:9">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>9</v>
       </c>
@@ -3242,10 +3295,10 @@
         <v>24</v>
       </c>
       <c r="I96">
-        <v>0.3391</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9">
+        <v>0.33910000000000001</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>9</v>
       </c>
@@ -3271,10 +3324,10 @@
         <v>24</v>
       </c>
       <c r="I97">
-        <v>0.267</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9">
+        <v>0.26700000000000002</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>9</v>
       </c>
@@ -3300,10 +3353,10 @@
         <v>24</v>
       </c>
       <c r="I98">
-        <v>0.333</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9">
+        <v>0.33300000000000002</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>10</v>
       </c>
@@ -3332,7 +3385,7 @@
         <v>0.2999</v>
       </c>
     </row>
-    <row r="100" spans="1:9">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>10</v>
       </c>
@@ -3358,10 +3411,10 @@
         <v>24</v>
       </c>
       <c r="I100">
-        <v>0.2659</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9">
+        <v>0.26590000000000003</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>10</v>
       </c>
@@ -3387,10 +3440,10 @@
         <v>24</v>
       </c>
       <c r="I101">
-        <v>0.325</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9">
+        <v>0.32500000000000001</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>9</v>
       </c>
@@ -3419,7 +3472,7 @@
         <v>0.2989</v>
       </c>
     </row>
-    <row r="103" spans="1:9">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>9</v>
       </c>
@@ -3448,7 +3501,7 @@
         <v>0.221</v>
       </c>
     </row>
-    <row r="104" spans="1:9">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>9</v>
       </c>
@@ -3474,10 +3527,10 @@
         <v>24</v>
       </c>
       <c r="I104">
-        <v>0.2919</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9">
+        <v>0.29189999999999999</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>10</v>
       </c>
@@ -3503,10 +3556,10 @@
         <v>24</v>
       </c>
       <c r="I105">
-        <v>0.2609</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9">
+        <v>0.26090000000000002</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>10</v>
       </c>
@@ -3532,10 +3585,10 @@
         <v>24</v>
       </c>
       <c r="I106">
-        <v>0.326</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9">
+        <v>0.32600000000000001</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>10</v>
       </c>
@@ -3561,10 +3614,10 @@
         <v>24</v>
       </c>
       <c r="I107">
-        <v>0.367</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9">
+        <v>0.36699999999999999</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>9</v>
       </c>
@@ -3590,10 +3643,10 @@
         <v>24</v>
       </c>
       <c r="I108">
-        <v>0.132999</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9">
+        <v>0.13299900000000001</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>9</v>
       </c>
@@ -3619,10 +3672,10 @@
         <v>24</v>
       </c>
       <c r="I109">
-        <v>0.295999</v>
-      </c>
-    </row>
-    <row r="110" spans="1:9">
+        <v>0.29599900000000001</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>9</v>
       </c>
@@ -3648,10 +3701,10 @@
         <v>24</v>
       </c>
       <c r="I110">
-        <v>0.332999</v>
-      </c>
-    </row>
-    <row r="111" spans="1:9">
+        <v>0.33299899999999999</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>9</v>
       </c>
@@ -3680,7 +3733,7 @@
         <v>0.527999</v>
       </c>
     </row>
-    <row r="112" spans="1:9">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>9</v>
       </c>
@@ -3709,7 +3762,7 @@
         <v>0.439</v>
       </c>
     </row>
-    <row r="113" spans="1:9">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>9</v>
       </c>
@@ -3735,10 +3788,10 @@
         <v>24</v>
       </c>
       <c r="I113">
-        <v>0.362</v>
-      </c>
-    </row>
-    <row r="114" spans="1:9">
+        <v>0.36199999999999999</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>10</v>
       </c>
@@ -3764,10 +3817,10 @@
         <v>24</v>
       </c>
       <c r="I114">
-        <v>0.364</v>
-      </c>
-    </row>
-    <row r="115" spans="1:9">
+        <v>0.36399999999999999</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>10</v>
       </c>
@@ -3793,10 +3846,10 @@
         <v>24</v>
       </c>
       <c r="I115">
-        <v>0.462</v>
-      </c>
-    </row>
-    <row r="116" spans="1:9">
+        <v>0.46200000000000002</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>10</v>
       </c>
@@ -3822,10 +3875,10 @@
         <v>24</v>
       </c>
       <c r="I116">
-        <v>0.462</v>
-      </c>
-    </row>
-    <row r="117" spans="1:9">
+        <v>0.46200000000000002</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>10</v>
       </c>
@@ -3854,7 +3907,7 @@
         <v>0.527999</v>
       </c>
     </row>
-    <row r="118" spans="1:9">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>9</v>
       </c>
@@ -3880,10 +3933,10 @@
         <v>24</v>
       </c>
       <c r="I118">
-        <v>0.329</v>
-      </c>
-    </row>
-    <row r="119" spans="1:9">
+        <v>0.32900000000000001</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>9</v>
       </c>
@@ -3909,10 +3962,10 @@
         <v>24</v>
       </c>
       <c r="I119">
-        <v>0.428999</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9">
+        <v>0.42899900000000002</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>9</v>
       </c>
@@ -3938,10 +3991,10 @@
         <v>24</v>
       </c>
       <c r="I120">
-        <v>0.461999</v>
-      </c>
-    </row>
-    <row r="121" spans="1:9">
+        <v>0.46199899999999999</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>10</v>
       </c>
@@ -3967,10 +4020,10 @@
         <v>24</v>
       </c>
       <c r="I121">
-        <v>0.495999</v>
-      </c>
-    </row>
-    <row r="122" spans="1:9">
+        <v>0.49599900000000002</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>10</v>
       </c>
@@ -3996,10 +4049,10 @@
         <v>24</v>
       </c>
       <c r="I122">
-        <v>0.496999</v>
-      </c>
-    </row>
-    <row r="123" spans="1:9">
+        <v>0.49699900000000002</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>10</v>
       </c>
@@ -4028,7 +4081,7 @@
         <v>0.402999</v>
       </c>
     </row>
-    <row r="124" spans="1:9">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>9</v>
       </c>
@@ -4054,10 +4107,10 @@
         <v>25</v>
       </c>
       <c r="I124">
-        <v>0.301</v>
-      </c>
-    </row>
-    <row r="125" spans="1:9">
+        <v>0.30099999999999999</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>9</v>
       </c>
@@ -4083,10 +4136,10 @@
         <v>25</v>
       </c>
       <c r="I125">
-        <v>0.267</v>
-      </c>
-    </row>
-    <row r="126" spans="1:9">
+        <v>0.26700000000000002</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>9</v>
       </c>
@@ -4112,10 +4165,10 @@
         <v>25</v>
       </c>
       <c r="I126">
-        <v>0.2899999</v>
-      </c>
-    </row>
-    <row r="127" spans="1:9">
+        <v>0.28999989999999998</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>9</v>
       </c>
@@ -4141,10 +4194,10 @@
         <v>25</v>
       </c>
       <c r="I127">
-        <v>0.362</v>
-      </c>
-    </row>
-    <row r="128" spans="1:9">
+        <v>0.36199999999999999</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>9</v>
       </c>
@@ -4170,10 +4223,10 @@
         <v>25</v>
       </c>
       <c r="I128">
-        <v>0.296999</v>
-      </c>
-    </row>
-    <row r="129" spans="1:9">
+        <v>0.29699900000000001</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>9</v>
       </c>
@@ -4199,10 +4252,10 @@
         <v>25</v>
       </c>
       <c r="I129">
-        <v>0.298999</v>
-      </c>
-    </row>
-    <row r="130" spans="1:9">
+        <v>0.29899900000000001</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>9</v>
       </c>
@@ -4228,10 +4281,10 @@
         <v>25</v>
       </c>
       <c r="I130">
-        <v>0.383999</v>
-      </c>
-    </row>
-    <row r="131" spans="1:9">
+        <v>0.38399899999999998</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>9</v>
       </c>
@@ -4257,10 +4310,10 @@
         <v>25</v>
       </c>
       <c r="I131">
-        <v>0.361</v>
-      </c>
-    </row>
-    <row r="132" spans="1:9">
+        <v>0.36099999999999999</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>9</v>
       </c>
@@ -4286,10 +4339,10 @@
         <v>25</v>
       </c>
       <c r="I132">
-        <v>0.428</v>
-      </c>
-    </row>
-    <row r="133" spans="1:9">
+        <v>0.42799999999999999</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>10</v>
       </c>
@@ -4315,10 +4368,10 @@
         <v>25</v>
       </c>
       <c r="I133">
-        <v>0.329999</v>
-      </c>
-    </row>
-    <row r="134" spans="1:9">
+        <v>0.32999899999999999</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>10</v>
       </c>
@@ -4344,10 +4397,10 @@
         <v>25</v>
       </c>
       <c r="I134">
-        <v>0.362999</v>
-      </c>
-    </row>
-    <row r="135" spans="1:9">
+        <v>0.36299900000000002</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>10</v>
       </c>
@@ -4373,10 +4426,10 @@
         <v>25</v>
       </c>
       <c r="I135">
-        <v>0.364999</v>
-      </c>
-    </row>
-    <row r="136" spans="1:9">
+        <v>0.36499900000000002</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>10</v>
       </c>
@@ -4405,7 +4458,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="137" spans="1:9">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>10</v>
       </c>
@@ -4434,7 +4487,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="138" spans="1:9">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>10</v>
       </c>
@@ -4460,10 +4513,10 @@
         <v>25</v>
       </c>
       <c r="I138">
-        <v>0.261</v>
-      </c>
-    </row>
-    <row r="139" spans="1:9">
+        <v>0.26100000000000001</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>9</v>
       </c>
@@ -4489,10 +4542,10 @@
         <v>25</v>
       </c>
       <c r="I139">
-        <v>0.265999</v>
-      </c>
-    </row>
-    <row r="140" spans="1:9">
+        <v>0.26599899999999999</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>9</v>
       </c>
@@ -4518,10 +4571,10 @@
         <v>25</v>
       </c>
       <c r="I140">
-        <v>0.362999</v>
-      </c>
-    </row>
-    <row r="141" spans="1:9">
+        <v>0.36299900000000002</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>9</v>
       </c>
@@ -4547,10 +4600,10 @@
         <v>25</v>
       </c>
       <c r="I141">
-        <v>0.358</v>
-      </c>
-    </row>
-    <row r="142" spans="1:9">
+        <v>0.35799999999999998</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>10</v>
       </c>
@@ -4576,10 +4629,10 @@
         <v>25</v>
       </c>
       <c r="I142">
-        <v>0.362999</v>
-      </c>
-    </row>
-    <row r="143" spans="1:9">
+        <v>0.36299900000000002</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>10</v>
       </c>
@@ -4605,10 +4658,10 @@
         <v>25</v>
       </c>
       <c r="I143">
-        <v>0.397999</v>
-      </c>
-    </row>
-    <row r="144" spans="1:9">
+        <v>0.39799899999999999</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>10</v>
       </c>
@@ -4634,10 +4687,10 @@
         <v>25</v>
       </c>
       <c r="I144">
-        <v>1.2408</v>
-      </c>
-    </row>
-    <row r="145" spans="1:9">
+        <v>1.2407999999999999</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>10</v>
       </c>
@@ -4663,10 +4716,10 @@
         <v>25</v>
       </c>
       <c r="I145">
-        <v>0.362999</v>
-      </c>
-    </row>
-    <row r="146" spans="1:9">
+        <v>0.36299900000000002</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>10</v>
       </c>
@@ -4692,10 +4745,10 @@
         <v>25</v>
       </c>
       <c r="I146">
-        <v>0.397999</v>
-      </c>
-    </row>
-    <row r="147" spans="1:9">
+        <v>0.39799899999999999</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>10</v>
       </c>
@@ -4721,10 +4774,10 @@
         <v>25</v>
       </c>
       <c r="I147">
-        <v>1.2408</v>
-      </c>
-    </row>
-    <row r="148" spans="1:9">
+        <v>1.2407999999999999</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>10</v>
       </c>
@@ -4750,10 +4803,10 @@
         <v>25</v>
       </c>
       <c r="I148">
-        <v>0.333999</v>
-      </c>
-    </row>
-    <row r="149" spans="1:9">
+        <v>0.33399899999999999</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>10</v>
       </c>
@@ -4782,7 +4835,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="150" spans="1:9">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>10</v>
       </c>
@@ -4808,10 +4861,10 @@
         <v>25</v>
       </c>
       <c r="I150">
-        <v>0.329</v>
-      </c>
-    </row>
-    <row r="151" spans="1:9">
+        <v>0.32900000000000001</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>9</v>
       </c>
@@ -4837,10 +4890,10 @@
         <v>25</v>
       </c>
       <c r="I151">
-        <v>0.3329</v>
-      </c>
-    </row>
-    <row r="152" spans="1:9">
+        <v>0.33289999999999997</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>9</v>
       </c>
@@ -4869,7 +4922,7 @@
         <v>0.2319</v>
       </c>
     </row>
-    <row r="153" spans="1:9">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>9</v>
       </c>
@@ -4898,7 +4951,7 @@
         <v>0.2969</v>
       </c>
     </row>
-    <row r="154" spans="1:9">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>10</v>
       </c>
@@ -4924,10 +4977,10 @@
         <v>25</v>
       </c>
       <c r="I154">
-        <v>0.4009</v>
-      </c>
-    </row>
-    <row r="155" spans="1:9">
+        <v>0.40089999999999998</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>10</v>
       </c>
@@ -4953,10 +5006,10 @@
         <v>25</v>
       </c>
       <c r="I155">
-        <v>0.233</v>
-      </c>
-    </row>
-    <row r="156" spans="1:9">
+        <v>0.23300000000000001</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>10</v>
       </c>
@@ -4982,10 +5035,10 @@
         <v>25</v>
       </c>
       <c r="I156">
-        <v>0.362</v>
-      </c>
-    </row>
-    <row r="157" spans="1:9">
+        <v>0.36199999999999999</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>9</v>
       </c>
@@ -5014,7 +5067,7 @@
         <v>0.3619</v>
       </c>
     </row>
-    <row r="158" spans="1:9">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>9</v>
       </c>
@@ -5040,10 +5093,10 @@
         <v>25</v>
       </c>
       <c r="I158">
-        <v>0.267</v>
-      </c>
-    </row>
-    <row r="159" spans="1:9">
+        <v>0.26700000000000002</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>9</v>
       </c>
@@ -5069,10 +5122,10 @@
         <v>25</v>
       </c>
       <c r="I159">
-        <v>0.3249</v>
-      </c>
-    </row>
-    <row r="160" spans="1:9">
+        <v>0.32490000000000002</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>10</v>
       </c>
@@ -5098,10 +5151,10 @@
         <v>25</v>
       </c>
       <c r="I160">
-        <v>0.301</v>
-      </c>
-    </row>
-    <row r="161" spans="1:9">
+        <v>0.30099999999999999</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>10</v>
       </c>
@@ -5127,10 +5180,10 @@
         <v>25</v>
       </c>
       <c r="I161">
-        <v>0.261</v>
-      </c>
-    </row>
-    <row r="162" spans="1:9">
+        <v>0.26100000000000001</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>10</v>
       </c>
@@ -5159,7 +5212,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="163" spans="1:9">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>9</v>
       </c>
@@ -5185,10 +5238,10 @@
         <v>25</v>
       </c>
       <c r="I163">
-        <v>0.2909</v>
-      </c>
-    </row>
-    <row r="164" spans="1:9">
+        <v>0.29089999999999999</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>9</v>
       </c>
@@ -5214,10 +5267,10 @@
         <v>25</v>
       </c>
       <c r="I164">
-        <v>0.2259</v>
-      </c>
-    </row>
-    <row r="165" spans="1:9">
+        <v>0.22589999999999999</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>9</v>
       </c>
@@ -5246,7 +5299,7 @@
         <v>0.108</v>
       </c>
     </row>
-    <row r="166" spans="1:9">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>10</v>
       </c>
@@ -5275,7 +5328,7 @@
         <v>0.2999</v>
       </c>
     </row>
-    <row r="167" spans="1:9">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>10</v>
       </c>
@@ -5301,10 +5354,10 @@
         <v>25</v>
       </c>
       <c r="I167">
-        <v>0.229</v>
-      </c>
-    </row>
-    <row r="168" spans="1:9">
+        <v>0.22900000000000001</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>10</v>
       </c>
@@ -5333,7 +5386,7 @@
         <v>0.2969</v>
       </c>
     </row>
-    <row r="169" spans="1:9">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>9</v>
       </c>
@@ -5359,10 +5412,10 @@
         <v>25</v>
       </c>
       <c r="I169">
-        <v>0.332999</v>
-      </c>
-    </row>
-    <row r="170" spans="1:9">
+        <v>0.33299899999999999</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>9</v>
       </c>
@@ -5388,10 +5441,10 @@
         <v>25</v>
       </c>
       <c r="I170">
-        <v>0.299999</v>
-      </c>
-    </row>
-    <row r="171" spans="1:9">
+        <v>0.29999900000000002</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>9</v>
       </c>
@@ -5417,10 +5470,10 @@
         <v>25</v>
       </c>
       <c r="I171">
-        <v>0.366999</v>
-      </c>
-    </row>
-    <row r="172" spans="1:9">
+        <v>0.36699900000000002</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>9</v>
       </c>
@@ -5449,7 +5502,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="173" spans="1:9">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>9</v>
       </c>
@@ -5475,10 +5528,10 @@
         <v>25</v>
       </c>
       <c r="I173">
-        <v>0.462</v>
-      </c>
-    </row>
-    <row r="174" spans="1:9">
+        <v>0.46200000000000002</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>9</v>
       </c>
@@ -5504,10 +5557,10 @@
         <v>25</v>
       </c>
       <c r="I174">
-        <v>0.296999</v>
-      </c>
-    </row>
-    <row r="175" spans="1:9">
+        <v>0.29699900000000001</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>10</v>
       </c>
@@ -5533,10 +5586,10 @@
         <v>25</v>
       </c>
       <c r="I175">
-        <v>0.528</v>
-      </c>
-    </row>
-    <row r="176" spans="1:9">
+        <v>0.52800000000000002</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>10</v>
       </c>
@@ -5562,10 +5615,10 @@
         <v>25</v>
       </c>
       <c r="I176">
-        <v>0.461999</v>
-      </c>
-    </row>
-    <row r="177" spans="1:9">
+        <v>0.46199899999999999</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>10</v>
       </c>
@@ -5591,10 +5644,10 @@
         <v>25</v>
       </c>
       <c r="I177">
-        <v>0.461999</v>
-      </c>
-    </row>
-    <row r="178" spans="1:9">
+        <v>0.46199899999999999</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>10</v>
       </c>
@@ -5620,10 +5673,10 @@
         <v>25</v>
       </c>
       <c r="I178">
-        <v>0.432999</v>
-      </c>
-    </row>
-    <row r="179" spans="1:9">
+        <v>0.43299900000000002</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>9</v>
       </c>
@@ -5649,10 +5702,10 @@
         <v>25</v>
       </c>
       <c r="I179">
-        <v>0.363999</v>
-      </c>
-    </row>
-    <row r="180" spans="1:9">
+        <v>0.36399900000000002</v>
+      </c>
+    </row>
+    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>9</v>
       </c>
@@ -5678,10 +5731,10 @@
         <v>25</v>
       </c>
       <c r="I180">
-        <v>0.429</v>
-      </c>
-    </row>
-    <row r="181" spans="1:9">
+        <v>0.42899999999999999</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>9</v>
       </c>
@@ -5707,10 +5760,10 @@
         <v>25</v>
       </c>
       <c r="I181">
-        <v>0.429999</v>
-      </c>
-    </row>
-    <row r="182" spans="1:9">
+        <v>0.42999900000000002</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>10</v>
       </c>
@@ -5736,10 +5789,10 @@
         <v>25</v>
       </c>
       <c r="I182">
-        <v>0.527</v>
-      </c>
-    </row>
-    <row r="183" spans="1:9">
+        <v>0.52700000000000002</v>
+      </c>
+    </row>
+    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>10</v>
       </c>
@@ -5765,10 +5818,10 @@
         <v>25</v>
       </c>
       <c r="I183">
-        <v>0.463</v>
-      </c>
-    </row>
-    <row r="184" spans="1:9">
+        <v>0.46300000000000002</v>
+      </c>
+    </row>
+    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>10</v>
       </c>
@@ -5797,7 +5850,7 @@
         <v>0.436</v>
       </c>
     </row>
-    <row r="185" spans="1:9">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>9</v>
       </c>
@@ -5823,10 +5876,10 @@
         <v>26</v>
       </c>
       <c r="I185">
-        <v>0.2289999</v>
-      </c>
-    </row>
-    <row r="186" spans="1:9">
+        <v>0.22899990000000001</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>9</v>
       </c>
@@ -5852,10 +5905,10 @@
         <v>26</v>
       </c>
       <c r="I186">
-        <v>0.231</v>
-      </c>
-    </row>
-    <row r="187" spans="1:9">
+        <v>0.23100000000000001</v>
+      </c>
+    </row>
+    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>9</v>
       </c>
@@ -5881,10 +5934,10 @@
         <v>26</v>
       </c>
       <c r="I187">
-        <v>0.266</v>
-      </c>
-    </row>
-    <row r="188" spans="1:9">
+        <v>0.26600000000000001</v>
+      </c>
+    </row>
+    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>9</v>
       </c>
@@ -5910,10 +5963,10 @@
         <v>26</v>
       </c>
       <c r="I188">
-        <v>0.329</v>
-      </c>
-    </row>
-    <row r="189" spans="1:9">
+        <v>0.32900000000000001</v>
+      </c>
+    </row>
+    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>9</v>
       </c>
@@ -5939,10 +5992,10 @@
         <v>26</v>
       </c>
       <c r="I189">
-        <v>0.331</v>
-      </c>
-    </row>
-    <row r="190" spans="1:9">
+        <v>0.33100000000000002</v>
+      </c>
+    </row>
+    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>9</v>
       </c>
@@ -5968,10 +6021,10 @@
         <v>26</v>
       </c>
       <c r="I190">
-        <v>0.329999</v>
-      </c>
-    </row>
-    <row r="191" spans="1:9">
+        <v>0.32999899999999999</v>
+      </c>
+    </row>
+    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>9</v>
       </c>
@@ -5997,10 +6050,10 @@
         <v>26</v>
       </c>
       <c r="I191">
-        <v>0.295</v>
-      </c>
-    </row>
-    <row r="192" spans="1:9">
+        <v>0.29499999999999998</v>
+      </c>
+    </row>
+    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>9</v>
       </c>
@@ -6026,10 +6079,10 @@
         <v>26</v>
       </c>
       <c r="I192">
-        <v>0.362999</v>
-      </c>
-    </row>
-    <row r="193" spans="1:9">
+        <v>0.36299900000000002</v>
+      </c>
+    </row>
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>9</v>
       </c>
@@ -6055,10 +6108,10 @@
         <v>26</v>
       </c>
       <c r="I193">
-        <v>0.825</v>
-      </c>
-    </row>
-    <row r="194" spans="1:9">
+        <v>0.82499999999999996</v>
+      </c>
+    </row>
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>10</v>
       </c>
@@ -6084,10 +6137,10 @@
         <v>26</v>
       </c>
       <c r="I194">
-        <v>0.328</v>
-      </c>
-    </row>
-    <row r="195" spans="1:9">
+        <v>0.32800000000000001</v>
+      </c>
+    </row>
+    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>10</v>
       </c>
@@ -6113,10 +6166,10 @@
         <v>26</v>
       </c>
       <c r="I195">
-        <v>0.364</v>
-      </c>
-    </row>
-    <row r="196" spans="1:9">
+        <v>0.36399999999999999</v>
+      </c>
+    </row>
+    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>10</v>
       </c>
@@ -6142,10 +6195,10 @@
         <v>26</v>
       </c>
       <c r="I196">
-        <v>0.328999</v>
-      </c>
-    </row>
-    <row r="197" spans="1:9">
+        <v>0.32899899999999999</v>
+      </c>
+    </row>
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>10</v>
       </c>
@@ -6171,10 +6224,10 @@
         <v>26</v>
       </c>
       <c r="I197">
-        <v>0.329</v>
-      </c>
-    </row>
-    <row r="198" spans="1:9">
+        <v>0.32900000000000001</v>
+      </c>
+    </row>
+    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>10</v>
       </c>
@@ -6200,10 +6253,10 @@
         <v>26</v>
       </c>
       <c r="I198">
-        <v>0.329</v>
-      </c>
-    </row>
-    <row r="199" spans="1:9">
+        <v>0.32900000000000001</v>
+      </c>
+    </row>
+    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>10</v>
       </c>
@@ -6229,10 +6282,10 @@
         <v>26</v>
       </c>
       <c r="I199">
-        <v>0.329999</v>
-      </c>
-    </row>
-    <row r="200" spans="1:9">
+        <v>0.32999899999999999</v>
+      </c>
+    </row>
+    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>9</v>
       </c>
@@ -6261,7 +6314,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="201" spans="1:9">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>9</v>
       </c>
@@ -6287,10 +6340,10 @@
         <v>26</v>
       </c>
       <c r="I201">
-        <v>0.463</v>
-      </c>
-    </row>
-    <row r="202" spans="1:9">
+        <v>0.46300000000000002</v>
+      </c>
+    </row>
+    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>9</v>
       </c>
@@ -6316,10 +6369,10 @@
         <v>26</v>
       </c>
       <c r="I202">
-        <v>0.396</v>
-      </c>
-    </row>
-    <row r="203" spans="1:9">
+        <v>0.39600000000000002</v>
+      </c>
+    </row>
+    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>10</v>
       </c>
@@ -6345,10 +6398,10 @@
         <v>26</v>
       </c>
       <c r="I203">
-        <v>0.329999</v>
-      </c>
-    </row>
-    <row r="204" spans="1:9">
+        <v>0.32999899999999999</v>
+      </c>
+    </row>
+    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>10</v>
       </c>
@@ -6374,10 +6427,10 @@
         <v>26</v>
       </c>
       <c r="I204">
-        <v>0.430999</v>
-      </c>
-    </row>
-    <row r="205" spans="1:9">
+        <v>0.43099900000000002</v>
+      </c>
+    </row>
+    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>10</v>
       </c>
@@ -6403,10 +6456,10 @@
         <v>26</v>
       </c>
       <c r="I205">
-        <v>0.750999</v>
-      </c>
-    </row>
-    <row r="206" spans="1:9">
+        <v>0.75099899999999997</v>
+      </c>
+    </row>
+    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>10</v>
       </c>
@@ -6432,10 +6485,10 @@
         <v>26</v>
       </c>
       <c r="I206">
-        <v>0.329999</v>
-      </c>
-    </row>
-    <row r="207" spans="1:9">
+        <v>0.32999899999999999</v>
+      </c>
+    </row>
+    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>10</v>
       </c>
@@ -6461,10 +6514,10 @@
         <v>26</v>
       </c>
       <c r="I207">
-        <v>0.430999</v>
-      </c>
-    </row>
-    <row r="208" spans="1:9">
+        <v>0.43099900000000002</v>
+      </c>
+    </row>
+    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>10</v>
       </c>
@@ -6490,10 +6543,10 @@
         <v>26</v>
       </c>
       <c r="I208">
-        <v>0.750999</v>
-      </c>
-    </row>
-    <row r="209" spans="1:9">
+        <v>0.75099899999999997</v>
+      </c>
+    </row>
+    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>10</v>
       </c>
@@ -6519,10 +6572,10 @@
         <v>26</v>
       </c>
       <c r="I209">
-        <v>0.299999</v>
-      </c>
-    </row>
-    <row r="210" spans="1:9">
+        <v>0.29999900000000002</v>
+      </c>
+    </row>
+    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>10</v>
       </c>
@@ -6548,10 +6601,10 @@
         <v>26</v>
       </c>
       <c r="I210">
-        <v>0.296999</v>
-      </c>
-    </row>
-    <row r="211" spans="1:9">
+        <v>0.29699900000000001</v>
+      </c>
+    </row>
+    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>10</v>
       </c>
@@ -6577,10 +6630,10 @@
         <v>26</v>
       </c>
       <c r="I211">
-        <v>0.298</v>
-      </c>
-    </row>
-    <row r="212" spans="1:9">
+        <v>0.29799999999999999</v>
+      </c>
+    </row>
+    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>9</v>
       </c>
@@ -6606,10 +6659,10 @@
         <v>26</v>
       </c>
       <c r="I212">
-        <v>0.3239</v>
-      </c>
-    </row>
-    <row r="213" spans="1:9">
+        <v>0.32390000000000002</v>
+      </c>
+    </row>
+    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>9</v>
       </c>
@@ -6635,10 +6688,10 @@
         <v>26</v>
       </c>
       <c r="I213">
-        <v>0.2679</v>
-      </c>
-    </row>
-    <row r="214" spans="1:9">
+        <v>0.26790000000000003</v>
+      </c>
+    </row>
+    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>9</v>
       </c>
@@ -6664,10 +6717,10 @@
         <v>26</v>
       </c>
       <c r="I214">
-        <v>0.233</v>
-      </c>
-    </row>
-    <row r="215" spans="1:9">
+        <v>0.23300000000000001</v>
+      </c>
+    </row>
+    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>10</v>
       </c>
@@ -6693,10 +6746,10 @@
         <v>26</v>
       </c>
       <c r="I215">
-        <v>0.3999</v>
-      </c>
-    </row>
-    <row r="216" spans="1:9">
+        <v>0.39989999999999998</v>
+      </c>
+    </row>
+    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>10</v>
       </c>
@@ -6722,10 +6775,10 @@
         <v>26</v>
       </c>
       <c r="I216">
-        <v>0.259</v>
-      </c>
-    </row>
-    <row r="217" spans="1:9">
+        <v>0.25900000000000001</v>
+      </c>
+    </row>
+    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>10</v>
       </c>
@@ -6751,10 +6804,10 @@
         <v>26</v>
       </c>
       <c r="I217">
-        <v>0.332</v>
-      </c>
-    </row>
-    <row r="218" spans="1:9">
+        <v>0.33200000000000002</v>
+      </c>
+    </row>
+    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>9</v>
       </c>
@@ -6780,10 +6833,10 @@
         <v>26</v>
       </c>
       <c r="I218">
-        <v>0.301</v>
-      </c>
-    </row>
-    <row r="219" spans="1:9">
+        <v>0.30099999999999999</v>
+      </c>
+    </row>
+    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>9</v>
       </c>
@@ -6809,10 +6862,10 @@
         <v>26</v>
       </c>
       <c r="I219">
-        <v>0.2659</v>
-      </c>
-    </row>
-    <row r="220" spans="1:9">
+        <v>0.26590000000000003</v>
+      </c>
+    </row>
+    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>9</v>
       </c>
@@ -6838,10 +6891,10 @@
         <v>26</v>
       </c>
       <c r="I220">
-        <v>0.2669</v>
-      </c>
-    </row>
-    <row r="221" spans="1:9">
+        <v>0.26690000000000003</v>
+      </c>
+    </row>
+    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>10</v>
       </c>
@@ -6867,10 +6920,10 @@
         <v>26</v>
       </c>
       <c r="I221">
-        <v>0.292</v>
-      </c>
-    </row>
-    <row r="222" spans="1:9">
+        <v>0.29199999999999998</v>
+      </c>
+    </row>
+    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>10</v>
       </c>
@@ -6896,10 +6949,10 @@
         <v>26</v>
       </c>
       <c r="I222">
-        <v>0.2599</v>
-      </c>
-    </row>
-    <row r="223" spans="1:9">
+        <v>0.25990000000000002</v>
+      </c>
+    </row>
+    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>10</v>
       </c>
@@ -6928,7 +6981,7 @@
         <v>0.3659</v>
       </c>
     </row>
-    <row r="224" spans="1:9">
+    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>9</v>
       </c>
@@ -6954,10 +7007,10 @@
         <v>26</v>
       </c>
       <c r="I224">
-        <v>0.364</v>
-      </c>
-    </row>
-    <row r="225" spans="1:9">
+        <v>0.36399999999999999</v>
+      </c>
+    </row>
+    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>9</v>
       </c>
@@ -6983,10 +7036,10 @@
         <v>26</v>
       </c>
       <c r="I225">
-        <v>0.234</v>
-      </c>
-    </row>
-    <row r="226" spans="1:9">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>9</v>
       </c>
@@ -7012,10 +7065,10 @@
         <v>26</v>
       </c>
       <c r="I226">
-        <v>0.2659</v>
-      </c>
-    </row>
-    <row r="227" spans="1:9">
+        <v>0.26590000000000003</v>
+      </c>
+    </row>
+    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>10</v>
       </c>
@@ -7041,10 +7094,10 @@
         <v>26</v>
       </c>
       <c r="I227">
-        <v>0.332</v>
-      </c>
-    </row>
-    <row r="228" spans="1:9">
+        <v>0.33200000000000002</v>
+      </c>
+    </row>
+    <row r="228" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>10</v>
       </c>
@@ -7073,7 +7126,7 @@
         <v>0.3019</v>
       </c>
     </row>
-    <row r="229" spans="1:9">
+    <row r="229" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>10</v>
       </c>
@@ -7099,10 +7152,10 @@
         <v>26</v>
       </c>
       <c r="I229">
-        <v>0.392</v>
-      </c>
-    </row>
-    <row r="230" spans="1:9">
+        <v>0.39200000000000002</v>
+      </c>
+    </row>
+    <row r="230" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>9</v>
       </c>
@@ -7128,10 +7181,10 @@
         <v>26</v>
       </c>
       <c r="I230">
-        <v>0.364</v>
-      </c>
-    </row>
-    <row r="231" spans="1:9">
+        <v>0.36399999999999999</v>
+      </c>
+    </row>
+    <row r="231" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>9</v>
       </c>
@@ -7160,7 +7213,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="232" spans="1:9">
+    <row r="232" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>9</v>
       </c>
@@ -7189,7 +7242,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="233" spans="1:9">
+    <row r="233" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>9</v>
       </c>
@@ -7215,10 +7268,10 @@
         <v>26</v>
       </c>
       <c r="I233">
-        <v>0.396</v>
-      </c>
-    </row>
-    <row r="234" spans="1:9">
+        <v>0.39600000000000002</v>
+      </c>
+    </row>
+    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>9</v>
       </c>
@@ -7244,10 +7297,10 @@
         <v>26</v>
       </c>
       <c r="I234">
-        <v>0.362999</v>
-      </c>
-    </row>
-    <row r="235" spans="1:9">
+        <v>0.36299900000000002</v>
+      </c>
+    </row>
+    <row r="235" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>9</v>
       </c>
@@ -7273,10 +7326,10 @@
         <v>26</v>
       </c>
       <c r="I235">
-        <v>0.295999</v>
-      </c>
-    </row>
-    <row r="236" spans="1:9">
+        <v>0.29599900000000001</v>
+      </c>
+    </row>
+    <row r="236" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>10</v>
       </c>
@@ -7302,10 +7355,10 @@
         <v>26</v>
       </c>
       <c r="I236">
-        <v>0.527</v>
-      </c>
-    </row>
-    <row r="237" spans="1:9">
+        <v>0.52700000000000002</v>
+      </c>
+    </row>
+    <row r="237" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>10</v>
       </c>
@@ -7331,10 +7384,10 @@
         <v>26</v>
       </c>
       <c r="I237">
-        <v>0.527</v>
-      </c>
-    </row>
-    <row r="238" spans="1:9">
+        <v>0.52700000000000002</v>
+      </c>
+    </row>
+    <row r="238" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>10</v>
       </c>
@@ -7360,10 +7413,10 @@
         <v>26</v>
       </c>
       <c r="I238">
-        <v>0.527</v>
-      </c>
-    </row>
-    <row r="239" spans="1:9">
+        <v>0.52700000000000002</v>
+      </c>
+    </row>
+    <row r="239" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>10</v>
       </c>
@@ -7389,10 +7442,10 @@
         <v>26</v>
       </c>
       <c r="I239">
-        <v>0.461999</v>
-      </c>
-    </row>
-    <row r="240" spans="1:9">
+        <v>0.46199899999999999</v>
+      </c>
+    </row>
+    <row r="240" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>9</v>
       </c>
@@ -7418,10 +7471,10 @@
         <v>26</v>
       </c>
       <c r="I240">
-        <v>0.362999</v>
-      </c>
-    </row>
-    <row r="241" spans="1:9">
+        <v>0.36299900000000002</v>
+      </c>
+    </row>
+    <row r="241" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>9</v>
       </c>
@@ -7447,10 +7500,10 @@
         <v>26</v>
       </c>
       <c r="I241">
-        <v>0.429</v>
-      </c>
-    </row>
-    <row r="242" spans="1:9">
+        <v>0.42899999999999999</v>
+      </c>
+    </row>
+    <row r="242" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>9</v>
       </c>
@@ -7476,10 +7529,10 @@
         <v>26</v>
       </c>
       <c r="I242">
-        <v>0.427999</v>
-      </c>
-    </row>
-    <row r="243" spans="1:9">
+        <v>0.42799900000000002</v>
+      </c>
+    </row>
+    <row r="243" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>10</v>
       </c>
@@ -7505,10 +7558,10 @@
         <v>26</v>
       </c>
       <c r="I243">
-        <v>0.725</v>
-      </c>
-    </row>
-    <row r="244" spans="1:9">
+        <v>0.72499999999999998</v>
+      </c>
+    </row>
+    <row r="244" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>10</v>
       </c>
@@ -7534,10 +7587,10 @@
         <v>26</v>
       </c>
       <c r="I244">
-        <v>0.428</v>
-      </c>
-    </row>
-    <row r="245" spans="1:9">
+        <v>0.42799999999999999</v>
+      </c>
+    </row>
+    <row r="245" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>10</v>
       </c>
@@ -7563,10 +7616,10 @@
         <v>26</v>
       </c>
       <c r="I245">
-        <v>0.333</v>
-      </c>
-    </row>
-    <row r="246" spans="1:9">
+        <v>0.33300000000000002</v>
+      </c>
+    </row>
+    <row r="246" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>9</v>
       </c>
@@ -7592,10 +7645,10 @@
         <v>27</v>
       </c>
       <c r="I246">
-        <v>0.267</v>
-      </c>
-    </row>
-    <row r="247" spans="1:9">
+        <v>0.26700000000000002</v>
+      </c>
+    </row>
+    <row r="247" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>9</v>
       </c>
@@ -7624,7 +7677,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="248" spans="1:9">
+    <row r="248" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>9</v>
       </c>
@@ -7650,10 +7703,10 @@
         <v>27</v>
       </c>
       <c r="I248">
-        <v>0.298999</v>
-      </c>
-    </row>
-    <row r="249" spans="1:9">
+        <v>0.29899900000000001</v>
+      </c>
+    </row>
+    <row r="249" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>9</v>
       </c>
@@ -7679,10 +7732,10 @@
         <v>27</v>
       </c>
       <c r="I249">
-        <v>0.329</v>
-      </c>
-    </row>
-    <row r="250" spans="1:9">
+        <v>0.32900000000000001</v>
+      </c>
+    </row>
+    <row r="250" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>9</v>
       </c>
@@ -7708,10 +7761,10 @@
         <v>27</v>
       </c>
       <c r="I250">
-        <v>0.26999</v>
-      </c>
-    </row>
-    <row r="251" spans="1:9">
+        <v>0.26999000000000001</v>
+      </c>
+    </row>
+    <row r="251" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>9</v>
       </c>
@@ -7737,10 +7790,10 @@
         <v>27</v>
       </c>
       <c r="I251">
-        <v>0.307999</v>
-      </c>
-    </row>
-    <row r="252" spans="1:9">
+        <v>0.30799900000000002</v>
+      </c>
+    </row>
+    <row r="252" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>9</v>
       </c>
@@ -7766,10 +7819,10 @@
         <v>27</v>
       </c>
       <c r="I252">
-        <v>0.431</v>
-      </c>
-    </row>
-    <row r="253" spans="1:9">
+        <v>0.43099999999999999</v>
+      </c>
+    </row>
+    <row r="253" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>9</v>
       </c>
@@ -7795,10 +7848,10 @@
         <v>27</v>
       </c>
       <c r="I253">
-        <v>0.264</v>
-      </c>
-    </row>
-    <row r="254" spans="1:9">
+        <v>0.26400000000000001</v>
+      </c>
+    </row>
+    <row r="254" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>9</v>
       </c>
@@ -7824,10 +7877,10 @@
         <v>27</v>
       </c>
       <c r="I254">
-        <v>1.055999</v>
-      </c>
-    </row>
-    <row r="255" spans="1:9">
+        <v>1.0559989999999999</v>
+      </c>
+    </row>
+    <row r="255" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>10</v>
       </c>
@@ -7853,10 +7906,10 @@
         <v>27</v>
       </c>
       <c r="I255">
-        <v>0.362999</v>
-      </c>
-    </row>
-    <row r="256" spans="1:9">
+        <v>0.36299900000000002</v>
+      </c>
+    </row>
+    <row r="256" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>10</v>
       </c>
@@ -7882,10 +7935,10 @@
         <v>27</v>
       </c>
       <c r="I256">
-        <v>0.332999</v>
-      </c>
-    </row>
-    <row r="257" spans="1:9">
+        <v>0.33299899999999999</v>
+      </c>
+    </row>
+    <row r="257" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>10</v>
       </c>
@@ -7914,7 +7967,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="258" spans="1:9">
+    <row r="258" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>10</v>
       </c>
@@ -7940,10 +7993,10 @@
         <v>27</v>
       </c>
       <c r="I258">
-        <v>0.361999</v>
-      </c>
-    </row>
-    <row r="259" spans="1:9">
+        <v>0.36199900000000002</v>
+      </c>
+    </row>
+    <row r="259" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>10</v>
       </c>
@@ -7969,10 +8022,10 @@
         <v>27</v>
       </c>
       <c r="I259">
-        <v>0.361999</v>
-      </c>
-    </row>
-    <row r="260" spans="1:9">
+        <v>0.36199900000000002</v>
+      </c>
+    </row>
+    <row r="260" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>10</v>
       </c>
@@ -7998,10 +8051,10 @@
         <v>27</v>
       </c>
       <c r="I260">
-        <v>0.268</v>
-      </c>
-    </row>
-    <row r="261" spans="1:9">
+        <v>0.26800000000000002</v>
+      </c>
+    </row>
+    <row r="261" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>9</v>
       </c>
@@ -8027,10 +8080,10 @@
         <v>27</v>
       </c>
       <c r="I261">
-        <v>0.362999</v>
-      </c>
-    </row>
-    <row r="262" spans="1:9">
+        <v>0.36299900000000002</v>
+      </c>
+    </row>
+    <row r="262" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>9</v>
       </c>
@@ -8059,7 +8112,7 @@
         <v>2.046999</v>
       </c>
     </row>
-    <row r="263" spans="1:9">
+    <row r="263" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>9</v>
       </c>
@@ -8085,10 +8138,10 @@
         <v>27</v>
       </c>
       <c r="I263">
-        <v>0.5949989999999999</v>
-      </c>
-    </row>
-    <row r="264" spans="1:9">
+        <v>0.59499899999999994</v>
+      </c>
+    </row>
+    <row r="264" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>10</v>
       </c>
@@ -8114,10 +8167,10 @@
         <v>27</v>
       </c>
       <c r="I264">
-        <v>0.5600000000000001</v>
-      </c>
-    </row>
-    <row r="265" spans="1:9">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="265" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>10</v>
       </c>
@@ -8143,10 +8196,10 @@
         <v>27</v>
       </c>
       <c r="I265">
-        <v>0.396</v>
-      </c>
-    </row>
-    <row r="266" spans="1:9">
+        <v>0.39600000000000002</v>
+      </c>
+    </row>
+    <row r="266" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>10</v>
       </c>
@@ -8172,10 +8225,10 @@
         <v>27</v>
       </c>
       <c r="I266">
-        <v>0.396</v>
-      </c>
-    </row>
-    <row r="267" spans="1:9">
+        <v>0.39600000000000002</v>
+      </c>
+    </row>
+    <row r="267" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>10</v>
       </c>
@@ -8201,10 +8254,10 @@
         <v>27</v>
       </c>
       <c r="I267">
-        <v>0.5600000000000001</v>
-      </c>
-    </row>
-    <row r="268" spans="1:9">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="268" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>10</v>
       </c>
@@ -8230,10 +8283,10 @@
         <v>27</v>
       </c>
       <c r="I268">
-        <v>0.396</v>
-      </c>
-    </row>
-    <row r="269" spans="1:9">
+        <v>0.39600000000000002</v>
+      </c>
+    </row>
+    <row r="269" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>10</v>
       </c>
@@ -8259,10 +8312,10 @@
         <v>27</v>
       </c>
       <c r="I269">
-        <v>0.396</v>
-      </c>
-    </row>
-    <row r="270" spans="1:9">
+        <v>0.39600000000000002</v>
+      </c>
+    </row>
+    <row r="270" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>10</v>
       </c>
@@ -8288,10 +8341,10 @@
         <v>27</v>
       </c>
       <c r="I270">
-        <v>0.433999</v>
-      </c>
-    </row>
-    <row r="271" spans="1:9">
+        <v>0.43399900000000002</v>
+      </c>
+    </row>
+    <row r="271" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>10</v>
       </c>
@@ -8317,10 +8370,10 @@
         <v>27</v>
       </c>
       <c r="I271">
-        <v>0.296999</v>
-      </c>
-    </row>
-    <row r="272" spans="1:9">
+        <v>0.29699900000000001</v>
+      </c>
+    </row>
+    <row r="272" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>10</v>
       </c>
@@ -8346,10 +8399,10 @@
         <v>27</v>
       </c>
       <c r="I272">
-        <v>0.362999</v>
-      </c>
-    </row>
-    <row r="273" spans="1:9">
+        <v>0.36299900000000002</v>
+      </c>
+    </row>
+    <row r="273" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>9</v>
       </c>
@@ -8378,7 +8431,7 @@
         <v>0.3649</v>
       </c>
     </row>
-    <row r="274" spans="1:9">
+    <row r="274" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>9</v>
       </c>
@@ -8404,10 +8457,10 @@
         <v>27</v>
       </c>
       <c r="I274">
-        <v>0.2259</v>
-      </c>
-    </row>
-    <row r="275" spans="1:9">
+        <v>0.22589999999999999</v>
+      </c>
+    </row>
+    <row r="275" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>9</v>
       </c>
@@ -8433,10 +8486,10 @@
         <v>27</v>
       </c>
       <c r="I275">
-        <v>0.264</v>
-      </c>
-    </row>
-    <row r="276" spans="1:9">
+        <v>0.26400000000000001</v>
+      </c>
+    </row>
+    <row r="276" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>10</v>
       </c>
@@ -8465,7 +8518,7 @@
         <v>0.3629</v>
       </c>
     </row>
-    <row r="277" spans="1:9">
+    <row r="277" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>10</v>
       </c>
@@ -8494,7 +8547,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="278" spans="1:9">
+    <row r="278" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>10</v>
       </c>
@@ -8520,10 +8573,10 @@
         <v>27</v>
       </c>
       <c r="I278">
-        <v>0.367</v>
-      </c>
-    </row>
-    <row r="279" spans="1:9">
+        <v>0.36699999999999999</v>
+      </c>
+    </row>
+    <row r="279" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>9</v>
       </c>
@@ -8549,10 +8602,10 @@
         <v>27</v>
       </c>
       <c r="I279">
-        <v>0.301</v>
-      </c>
-    </row>
-    <row r="280" spans="1:9">
+        <v>0.30099999999999999</v>
+      </c>
+    </row>
+    <row r="280" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>9</v>
       </c>
@@ -8578,10 +8631,10 @@
         <v>27</v>
       </c>
       <c r="I280">
-        <v>0.3249</v>
-      </c>
-    </row>
-    <row r="281" spans="1:9">
+        <v>0.32490000000000002</v>
+      </c>
+    </row>
+    <row r="281" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>9</v>
       </c>
@@ -8607,10 +8660,10 @@
         <v>27</v>
       </c>
       <c r="I281">
-        <v>0.267</v>
-      </c>
-    </row>
-    <row r="282" spans="1:9">
+        <v>0.26700000000000002</v>
+      </c>
+    </row>
+    <row r="282" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>10</v>
       </c>
@@ -8636,10 +8689,10 @@
         <v>27</v>
       </c>
       <c r="I282">
-        <v>0.3179</v>
-      </c>
-    </row>
-    <row r="283" spans="1:9">
+        <v>0.31790000000000002</v>
+      </c>
+    </row>
+    <row r="283" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>10</v>
       </c>
@@ -8665,10 +8718,10 @@
         <v>27</v>
       </c>
       <c r="I283">
-        <v>0.233</v>
-      </c>
-    </row>
-    <row r="284" spans="1:9">
+        <v>0.23300000000000001</v>
+      </c>
+    </row>
+    <row r="284" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>10</v>
       </c>
@@ -8697,7 +8750,7 @@
         <v>0.3589</v>
       </c>
     </row>
-    <row r="285" spans="1:9">
+    <row r="285" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>9</v>
       </c>
@@ -8726,7 +8779,7 @@
         <v>0.2999</v>
       </c>
     </row>
-    <row r="286" spans="1:9">
+    <row r="286" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>9</v>
       </c>
@@ -8755,7 +8808,7 @@
         <v>0.2319</v>
       </c>
     </row>
-    <row r="287" spans="1:9">
+    <row r="287" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>9</v>
       </c>
@@ -8781,10 +8834,10 @@
         <v>27</v>
       </c>
       <c r="I287">
-        <v>0.2569</v>
-      </c>
-    </row>
-    <row r="288" spans="1:9">
+        <v>0.25690000000000002</v>
+      </c>
+    </row>
+    <row r="288" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>10</v>
       </c>
@@ -8810,10 +8863,10 @@
         <v>27</v>
       </c>
       <c r="I288">
-        <v>0.359</v>
-      </c>
-    </row>
-    <row r="289" spans="1:9">
+        <v>0.35899999999999999</v>
+      </c>
+    </row>
+    <row r="289" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>10</v>
       </c>
@@ -8839,10 +8892,10 @@
         <v>27</v>
       </c>
       <c r="I289">
-        <v>0.257</v>
-      </c>
-    </row>
-    <row r="290" spans="1:9">
+        <v>0.25700000000000001</v>
+      </c>
+    </row>
+    <row r="290" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>10</v>
       </c>
@@ -8868,10 +8921,10 @@
         <v>27</v>
       </c>
       <c r="I290">
-        <v>0.397</v>
-      </c>
-    </row>
-    <row r="291" spans="1:9">
+        <v>0.39700000000000002</v>
+      </c>
+    </row>
+    <row r="291" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>9</v>
       </c>
@@ -8897,10 +8950,10 @@
         <v>27</v>
       </c>
       <c r="I291">
-        <v>0.332</v>
-      </c>
-    </row>
-    <row r="292" spans="1:9">
+        <v>0.33200000000000002</v>
+      </c>
+    </row>
+    <row r="292" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>9</v>
       </c>
@@ -8929,7 +8982,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="293" spans="1:9">
+    <row r="293" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>9</v>
       </c>
@@ -8955,10 +9008,10 @@
         <v>27</v>
       </c>
       <c r="I293">
-        <v>0.365999</v>
-      </c>
-    </row>
-    <row r="294" spans="1:9">
+        <v>0.36599900000000002</v>
+      </c>
+    </row>
+    <row r="294" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>9</v>
       </c>
@@ -8984,10 +9037,10 @@
         <v>27</v>
       </c>
       <c r="I294">
-        <v>0.364999</v>
-      </c>
-    </row>
-    <row r="295" spans="1:9">
+        <v>0.36499900000000002</v>
+      </c>
+    </row>
+    <row r="295" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>9</v>
       </c>
@@ -9016,7 +9069,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="296" spans="1:9">
+    <row r="296" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>9</v>
       </c>
@@ -9042,10 +9095,10 @@
         <v>27</v>
       </c>
       <c r="I296">
-        <v>0.362999</v>
-      </c>
-    </row>
-    <row r="297" spans="1:9">
+        <v>0.36299900000000002</v>
+      </c>
+    </row>
+    <row r="297" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>10</v>
       </c>
@@ -9071,10 +9124,10 @@
         <v>27</v>
       </c>
       <c r="I297">
-        <v>0.462999</v>
-      </c>
-    </row>
-    <row r="298" spans="1:9">
+        <v>0.46299899999999999</v>
+      </c>
+    </row>
+    <row r="298" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>10</v>
       </c>
@@ -9100,10 +9153,10 @@
         <v>27</v>
       </c>
       <c r="I298">
-        <v>0.362999</v>
-      </c>
-    </row>
-    <row r="299" spans="1:9">
+        <v>0.36299900000000002</v>
+      </c>
+    </row>
+    <row r="299" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>10</v>
       </c>
@@ -9129,10 +9182,10 @@
         <v>27</v>
       </c>
       <c r="I299">
-        <v>0.362999</v>
-      </c>
-    </row>
-    <row r="300" spans="1:9">
+        <v>0.36299900000000002</v>
+      </c>
+    </row>
+    <row r="300" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>10</v>
       </c>
@@ -9158,10 +9211,10 @@
         <v>27</v>
       </c>
       <c r="I300">
-        <v>0.429</v>
-      </c>
-    </row>
-    <row r="301" spans="1:9">
+        <v>0.42899999999999999</v>
+      </c>
+    </row>
+    <row r="301" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>9</v>
       </c>
@@ -9190,7 +9243,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="302" spans="1:9">
+    <row r="302" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>9</v>
       </c>
@@ -9216,10 +9269,10 @@
         <v>27</v>
       </c>
       <c r="I302">
-        <v>0.329</v>
-      </c>
-    </row>
-    <row r="303" spans="1:9">
+        <v>0.32900000000000001</v>
+      </c>
+    </row>
+    <row r="303" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>9</v>
       </c>
@@ -9245,10 +9298,10 @@
         <v>27</v>
       </c>
       <c r="I303">
-        <v>0.427999</v>
-      </c>
-    </row>
-    <row r="304" spans="1:9">
+        <v>0.42799900000000002</v>
+      </c>
+    </row>
+    <row r="304" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>10</v>
       </c>
@@ -9274,10 +9327,10 @@
         <v>27</v>
       </c>
       <c r="I304">
-        <v>0.493999</v>
-      </c>
-    </row>
-    <row r="305" spans="1:9">
+        <v>0.49399900000000002</v>
+      </c>
+    </row>
+    <row r="305" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>10</v>
       </c>
@@ -9303,10 +9356,10 @@
         <v>27</v>
       </c>
       <c r="I305">
-        <v>0.493999</v>
-      </c>
-    </row>
-    <row r="306" spans="1:9">
+        <v>0.49399900000000002</v>
+      </c>
+    </row>
+    <row r="306" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>10</v>
       </c>
@@ -9333,6 +9386,79 @@
       </c>
       <c r="I306">
         <v>0.533999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86E7278E-4BD8-4878-A231-09F1EE72E804}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>4973</v>
+      </c>
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2">
+        <v>0.29899900000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>